<commit_message>
1. created the begining of the Toaster GUI for arcpro 2. Edited the UOT tool to create relative hyperlinks rather than absolute 3. Redirected the AST Call Routine to call the new UOT tool with edited hyperlinks script, The old UOT Tool still remains as original
</commit_message>
<xml_diff>
--- a/autoast/auto_ast_V2_Cuisinart_MultiP_PdfMaps/2nd batch jobs.xlsx
+++ b/autoast/auto_ast_V2_Cuisinart_MultiP_PdfMaps/2nd batch jobs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="20">
   <si>
     <t>region</t>
   </si>
@@ -73,49 +73,7 @@
     <t>true</t>
   </si>
   <si>
-    <t>//spatialfiles.bcgov/work/srm/gss/projects/gr_2025_26_general_request_batch_20_statuses/work/Second Batch\139_south coast\139.shp</t>
-  </si>
-  <si>
-    <t>//spatialfiles.bcgov/work/srm/gss/projects/gr_2025_26_general_request_batch_20_statuses/work/Second Batch\outputs\139_south coast</t>
-  </si>
-  <si>
-    <t>//spatialfiles.bcgov/work/srm/gss/projects/gr_2025_26_general_request_batch_20_statuses/work/Second Batch\144_south coast\144.shp</t>
-  </si>
-  <si>
-    <t>//spatialfiles.bcgov/work/srm/gss/projects/gr_2025_26_general_request_batch_20_statuses/work/Second Batch\outputs\144_south coast</t>
-  </si>
-  <si>
-    <t>//spatialfiles.bcgov/work/srm/gss/projects/gr_2025_26_general_request_batch_20_statuses/work/Second Batch\151_south coast\151.shp</t>
-  </si>
-  <si>
-    <t>//spatialfiles.bcgov/work/srm/gss/projects/gr_2025_26_general_request_batch_20_statuses/work/Second Batch\outputs\151_south coast</t>
-  </si>
-  <si>
-    <t>//spatialfiles.bcgov/work/srm/gss/projects/gr_2025_26_general_request_batch_20_statuses/work/Second Batch\161_south coast\161.shp</t>
-  </si>
-  <si>
-    <t>//spatialfiles.bcgov/work/srm/gss/projects/gr_2025_26_general_request_batch_20_statuses/work/Second Batch\outputs\161_south coast</t>
-  </si>
-  <si>
-    <t>West_Coast</t>
-  </si>
-  <si>
-    <t>//spatialfiles.bcgov/work/srm/gss/projects/gr_2025_26_general_request_batch_20_statuses/work/Second Batch\192_west coast\192.shp</t>
-  </si>
-  <si>
-    <t>//spatialfiles.bcgov/work/srm/gss/projects/gr_2025_26_general_request_batch_20_statuses/work/Second Batch\outputs\192_west coast</t>
-  </si>
-  <si>
-    <t>//spatialfiles.bcgov/work/srm/gss/projects/gr_2025_26_general_request_batch_20_statuses/work/Second Batch\232_south coast\232.shp</t>
-  </si>
-  <si>
-    <t>//spatialfiles.bcgov/work/srm/gss/projects/gr_2025_26_general_request_batch_20_statuses/work/Second Batch\outputs\232_south coast</t>
-  </si>
-  <si>
-    <t>//spatialfiles.bcgov/work/srm/gss/projects/gr_2025_26_general_request_batch_20_statuses/work/Second Batch\237_south coast\237.shp</t>
-  </si>
-  <si>
-    <t>//spatialfiles.bcgov/work/srm/gss/projects/gr_2025_26_general_request_batch_20_statuses/work/Second Batch\outputs\237_south coast</t>
+    <t/>
   </si>
 </sst>
 </file>
@@ -123,13 +81,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -140,7 +104,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -152,12 +123,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -474,20 +451,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="64.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="154.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="64.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="154.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -569,239 +546,239 @@
       <c r="N2" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>18</v>
+      <c r="F3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>21</v>
+      <c r="A4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>18</v>
+      <c r="F4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>23</v>
+      <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>18</v>
+      <c r="F5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>25</v>
+      <c r="A6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>18</v>
+      <c r="F6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>28</v>
+      <c r="A7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>18</v>
+      <c r="F7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>30</v>
+      <c r="A8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>18</v>
+      <c r="F8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>32</v>
+      <c r="A9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>18</v>
+      <c r="F9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>

</xml_diff>